<commit_message>
Progres in lesson for 04-segment
</commit_message>
<xml_diff>
--- a/04-segment/Home_preparation-Truth_Table_for_7_segment_display.xlsx
+++ b/04-segment/Home_preparation-Truth_Table_for_7_segment_display.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Documents\DigitalElectronics1\04-segment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\240642\Documents\DigitalElectronics1\04-segment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBE2032F-2C85-4A6B-9EA6-261D6AF48C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9ADE32F-A44B-4C59-86AC-FD5163696CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FBE1E8C9-6168-412D-9142-8331AA8C4560}"/>
+    <workbookView xWindow="-9750" yWindow="840" windowWidth="21600" windowHeight="11385" xr2:uid="{FBE1E8C9-6168-412D-9142-8331AA8C4560}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -458,43 +458,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Čárka" xfId="1" builtinId="3"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -510,7 +539,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -809,502 +838,502 @@
   <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="18" t="s">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13" t="s">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14">
-        <v>0</v>
-      </c>
-      <c r="E3" s="15">
-        <v>0</v>
-      </c>
-      <c r="F3" s="15">
-        <v>0</v>
-      </c>
-      <c r="G3" s="15">
-        <v>0</v>
-      </c>
-      <c r="H3" s="15">
-        <v>0</v>
-      </c>
-      <c r="I3" s="15">
-        <v>0</v>
-      </c>
-      <c r="J3" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="9">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="9">
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
+        <v>1</v>
+      </c>
+      <c r="H4" s="14">
+        <v>1</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1</v>
+      </c>
+      <c r="J4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
         <v>2</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="9">
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1</v>
+      </c>
+      <c r="G5" s="14">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14">
+        <v>0</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="11">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="9">
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14">
+        <v>1</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="11">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="9">
+      <c r="D7" s="13">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0</v>
+      </c>
+      <c r="G7" s="14">
+        <v>1</v>
+      </c>
+      <c r="H7" s="14">
+        <v>1</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="11">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="9">
+      <c r="D8" s="13">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1</v>
+      </c>
+      <c r="F8" s="14">
+        <v>0</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="11">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="9">
+      <c r="D9" s="13">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14">
+        <v>0</v>
+      </c>
+      <c r="I9" s="14">
+        <v>0</v>
+      </c>
+      <c r="J9" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="11">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="9">
+      <c r="D10" s="13">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14">
+        <v>0</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1</v>
+      </c>
+      <c r="H10" s="14">
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
+        <v>1</v>
+      </c>
+      <c r="J10" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
         <v>8</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="5">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="9">
+      <c r="D11" s="13">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14">
+        <v>0</v>
+      </c>
+      <c r="I11" s="14">
+        <v>0</v>
+      </c>
+      <c r="J11" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
         <v>9</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="5">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="10" t="s">
+      <c r="D12" s="13">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14">
+        <v>0</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14">
+        <v>0</v>
+      </c>
+      <c r="J12" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="5">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="10" t="s">
+      <c r="D13" s="13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0</v>
+      </c>
+      <c r="G13" s="14">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14">
+        <v>0</v>
+      </c>
+      <c r="I13" s="14">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="10" t="s">
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="10" t="s">
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
+      <c r="J15" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>1</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="10" t="s">
+      <c r="D16" s="13">
+        <v>1</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="11" t="s">
+      <c r="D17" s="13">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
+        <v>1</v>
+      </c>
+      <c r="F17" s="14">
+        <v>1</v>
+      </c>
+      <c r="G17" s="14">
+        <v>0</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="3">
-        <v>1</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="D18" s="18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="19">
+        <v>1</v>
+      </c>
+      <c r="F18" s="19">
+        <v>1</v>
+      </c>
+      <c r="G18" s="19">
+        <v>1</v>
+      </c>
+      <c r="H18" s="19">
+        <v>0</v>
+      </c>
+      <c r="I18" s="19">
+        <v>0</v>
+      </c>
+      <c r="J18" s="20">
         <v>0</v>
       </c>
     </row>

</xml_diff>